<commit_message>
Update sector_mapping: add 7BC_Indirect-N2O
</commit_message>
<xml_diff>
--- a/data/national/ceds/data_aux/sector_mapping.xlsx
+++ b/data/national/ceds/data_aux/sector_mapping.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{4A42AE8B-B62B-0440-BF35-1D1907A656B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{617353F2-06B0-4562-ADB3-16C84A6BB53E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FC66F7-0C90-4553-89DD-00CE60E58CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="835" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="835" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sector_Mapping" sheetId="1" r:id="rId1"/>
@@ -2168,7 +2168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4796" uniqueCount="1991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4797" uniqueCount="1991">
   <si>
     <t>CEDS_59</t>
   </si>
@@ -34746,7 +34746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -36952,7 +36952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
@@ -38123,8 +38123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B58F7F-6C03-4642-B26B-B1CECDED4318}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39560,6 +39560,9 @@
       <c r="B65" s="188"/>
       <c r="C65" s="188"/>
       <c r="D65" s="186"/>
+      <c r="F65" s="10" t="s">
+        <v>175</v>
+      </c>
       <c r="G65" s="186" t="s">
         <v>1982</v>
       </c>
@@ -40896,7 +40899,7 @@
   <dimension ref="A1:M238"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C158" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C187" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F234" sqref="F234"/>

</xml_diff>